<commit_message>
Removed invalid PV from PLC
</commit_message>
<xml_diff>
--- a/etc/Storage Ring A Interlock EPICS.xlsx
+++ b/etc/Storage Ring A Interlock EPICS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23802"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3101695D-1059-4F80-B3B0-FDCD40C07F1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46E0969C-555B-4835-A1A1-CD688E099416}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSAmp Tower 04" sheetId="15" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6515" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6512" uniqueCount="657">
   <si>
     <t>Nº</t>
   </si>
@@ -27340,8 +27340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U105"/>
   <sheetViews>
-    <sheetView topLeftCell="B96" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="C77" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27355,7 +27355,7 @@
     <col min="10" max="10" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="44.28515625" customWidth="1"/>
     <col min="12" max="12" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.42578125" customWidth="1"/>
+    <col min="13" max="13" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.140625" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" customWidth="1"/>
@@ -33915,8 +33915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D9DEC3-FCCA-4464-9BBF-01B2481D03F0}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="J11" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34987,26 +34987,14 @@
       </c>
       <c r="K19" s="63"/>
       <c r="L19" s="63"/>
-      <c r="M19" s="64" t="str">
-        <f t="shared" si="1"/>
-        <v>RA_TLSIA_RF_Circulator_PwrRevIndBm_Mon</v>
-      </c>
-      <c r="N19" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="O19" s="64" t="s">
-        <v>30</v>
-      </c>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="64"/>
       <c r="P19" s="64"/>
       <c r="Q19" s="64"/>
       <c r="R19" s="64"/>
-      <c r="S19" s="64" t="str">
-        <f>M19</f>
-        <v>RA_TLSIA_RF_Circulator_PwrRevIndBm_Mon</v>
-      </c>
-      <c r="T19" s="64" t="s">
-        <v>52</v>
-      </c>
+      <c r="S19" s="64"/>
+      <c r="T19" s="64"/>
       <c r="U19" s="65"/>
     </row>
     <row r="20" spans="1:21" s="5" customFormat="1">
@@ -42631,8 +42619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A52F41C-E692-4BB3-8E5F-3C78FBFA71A0}">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Include TUp & TDown
</commit_message>
<xml_diff>
--- a/etc/Storage Ring A Interlock EPICS.xlsx
+++ b/etc/Storage Ring A Interlock EPICS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B75CD540-DBA6-4116-AFF1-F4AF81C32260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97578A0C-CB7E-4E7D-B27E-90179D98252F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="90" yWindow="1560" windowWidth="20400" windowHeight="9480" tabRatio="719" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6526" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6552" uniqueCount="665">
   <si>
     <t>Nº</t>
   </si>
@@ -1376,6 +1376,18 @@
   </si>
   <si>
     <t>Set_Temp[9]</t>
+  </si>
+  <si>
+    <t>PT - 100 Janela de Quartzo P7 Abaixo do Set</t>
+  </si>
+  <si>
+    <t>GlassWinTUp</t>
+  </si>
+  <si>
+    <t>PT - 100 Janela de Quartzo P7 Acima do Set</t>
+  </si>
+  <si>
+    <t>GlassWinTDown</t>
   </si>
   <si>
     <t>Disc 1 Water Temperature</t>
@@ -8518,8 +8530,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C14A82AC-8A8B-4AE6-8243-55496A5CEF7D}" name="Table9" displayName="Table9" ref="A1:U48" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100" headerRowBorderDxfId="98" tableBorderDxfId="99" totalsRowBorderDxfId="97">
-  <autoFilter ref="A1:U48" xr:uid="{7CB02FD4-FF14-4496-98B3-4F8B1299769D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C14A82AC-8A8B-4AE6-8243-55496A5CEF7D}" name="Table9" displayName="Table9" ref="A1:U50" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100" headerRowBorderDxfId="98" tableBorderDxfId="99" totalsRowBorderDxfId="97">
+  <autoFilter ref="A1:U50" xr:uid="{7CB02FD4-FF14-4496-98B3-4F8B1299769D}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{3D88C2FC-5174-41B4-A3FD-F1FA680784DE}" name="Nº" dataDxfId="96"/>
     <tableColumn id="2" xr3:uid="{05D8D350-F8D6-4479-AC39-69A78320DBEF}" name="Description" dataDxfId="95"/>
@@ -14837,27 +14849,27 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="4" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" s="2" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="3" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="4" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
     </row>
   </sheetData>
@@ -35187,7 +35199,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{188945DB-2545-476B-BE7E-6067BB31C627}">
-  <dimension ref="A1:U48"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L25" workbookViewId="0">
       <selection activeCell="Q49" sqref="Q49"/>
@@ -35195,7 +35207,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -38418,6 +38430,138 @@
       <c r="U48" s="44">
         <v>2</v>
       </c>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="A49" s="39">
+        <v>46</v>
+      </c>
+      <c r="B49" s="40" t="s">
+        <v>443</v>
+      </c>
+      <c r="C49" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="D49" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="E49" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="41" t="s">
+        <v>343</v>
+      </c>
+      <c r="G49" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H49" s="41" t="s">
+        <v>444</v>
+      </c>
+      <c r="I49" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="J49" s="42" t="str">
+        <f>IF(G49="-",C49&amp;"-"&amp;D49&amp;":"&amp;E49&amp;"-"&amp;F49&amp;":"&amp;H49&amp;"-"&amp;I49,C49&amp;"-"&amp;D49&amp;":"&amp;E49&amp;"-"&amp;F49&amp;"-"&amp;G49&amp;":"&amp;H49&amp;"-"&amp;I49)</f>
+        <v>SI-02SB:RF-P7Cav:GlassWinTUp-Mon</v>
+      </c>
+      <c r="K49" s="42" t="str">
+        <f>IF(OR(P49="",P49="N/A"),"N/A",IF(G49="-",C49&amp;"-"&amp;D49&amp;":"&amp;E49&amp;"-"&amp;F49&amp;":"&amp;H49&amp;"UpperLimit-Cte",C49&amp;"-"&amp;D49&amp;":"&amp;E49&amp;"-"&amp;F49&amp;"-"&amp;G49&amp;":"&amp;H49&amp;"UpperLimit-Cte"))</f>
+        <v>N/A</v>
+      </c>
+      <c r="L49" s="42" t="str">
+        <f>IF(OR(Q49="",Q49="N/A"),"N/A",IF(G49="-",C49&amp;"-"&amp;D49&amp;":"&amp;E49&amp;"-"&amp;F49&amp;":"&amp;H49&amp;"LowerLimit-Cte",C49&amp;"-"&amp;D49&amp;":"&amp;E49&amp;"-"&amp;F49&amp;"-"&amp;G49&amp;":"&amp;H49&amp;"LowerLimit-Cte"))</f>
+        <v>N/A</v>
+      </c>
+      <c r="M49" s="43" t="str">
+        <f>IF(G49="-",C49&amp;"_"&amp;D49&amp;"_"&amp;E49&amp;"_"&amp;F49&amp;"_"&amp;H49&amp;""&amp;I49,C49&amp;"_"&amp;D49&amp;"_"&amp;E49&amp;"_"&amp;F49&amp;"_"&amp;G49&amp;"_"&amp;H49&amp;""&amp;I49)</f>
+        <v>SI_02SB_RF_P7Cav_GlassWinTUpMon</v>
+      </c>
+      <c r="N49" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="O49" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P49" s="31" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q49" s="31" t="s">
+        <v>345</v>
+      </c>
+      <c r="R49" s="43"/>
+      <c r="S49" s="43" t="str">
+        <f>M49</f>
+        <v>SI_02SB_RF_P7Cav_GlassWinTUpMon</v>
+      </c>
+      <c r="T49" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="U49" s="44"/>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50" s="39">
+        <v>47</v>
+      </c>
+      <c r="B50" s="40" t="s">
+        <v>445</v>
+      </c>
+      <c r="C50" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="E50" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="41" t="s">
+        <v>343</v>
+      </c>
+      <c r="G50" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H50" s="41" t="s">
+        <v>446</v>
+      </c>
+      <c r="I50" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="J50" s="42" t="str">
+        <f>IF(G50="-",C50&amp;"-"&amp;D50&amp;":"&amp;E50&amp;"-"&amp;F50&amp;":"&amp;H50&amp;"-"&amp;I50,C50&amp;"-"&amp;D50&amp;":"&amp;E50&amp;"-"&amp;F50&amp;"-"&amp;G50&amp;":"&amp;H50&amp;"-"&amp;I50)</f>
+        <v>SI-02SB:RF-P7Cav:GlassWinTDown-Mon</v>
+      </c>
+      <c r="K50" s="42" t="str">
+        <f>IF(OR(P50="",P50="N/A"),"N/A",IF(G50="-",C50&amp;"-"&amp;D50&amp;":"&amp;E50&amp;"-"&amp;F50&amp;":"&amp;H50&amp;"UpperLimit-Cte",C50&amp;"-"&amp;D50&amp;":"&amp;E50&amp;"-"&amp;F50&amp;"-"&amp;G50&amp;":"&amp;H50&amp;"UpperLimit-Cte"))</f>
+        <v>N/A</v>
+      </c>
+      <c r="L50" s="42" t="str">
+        <f>IF(OR(Q50="",Q50="N/A"),"N/A",IF(G50="-",C50&amp;"-"&amp;D50&amp;":"&amp;E50&amp;"-"&amp;F50&amp;":"&amp;H50&amp;"LowerLimit-Cte",C50&amp;"-"&amp;D50&amp;":"&amp;E50&amp;"-"&amp;F50&amp;"-"&amp;G50&amp;":"&amp;H50&amp;"LowerLimit-Cte"))</f>
+        <v>N/A</v>
+      </c>
+      <c r="M50" s="43" t="str">
+        <f>IF(G50="-",C50&amp;"_"&amp;D50&amp;"_"&amp;E50&amp;"_"&amp;F50&amp;"_"&amp;H50&amp;""&amp;I50,C50&amp;"_"&amp;D50&amp;"_"&amp;E50&amp;"_"&amp;F50&amp;"_"&amp;G50&amp;"_"&amp;H50&amp;""&amp;I50)</f>
+        <v>SI_02SB_RF_P7Cav_GlassWinTDownMon</v>
+      </c>
+      <c r="N50" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="O50" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P50" s="71" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q50" s="71" t="s">
+        <v>345</v>
+      </c>
+      <c r="R50" s="43"/>
+      <c r="S50" s="43" t="str">
+        <f>M50</f>
+        <v>SI_02SB_RF_P7Cav_GlassWinTDownMon</v>
+      </c>
+      <c r="T50" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="U50" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -38522,7 +38666,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>242</v>
@@ -38540,7 +38684,7 @@
         <v>26</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>28</v>
@@ -38559,7 +38703,7 @@
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
       <c r="T2" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U2" s="18"/>
     </row>
@@ -38568,7 +38712,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>242</v>
@@ -38586,7 +38730,7 @@
         <v>26</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>28</v>
@@ -38605,7 +38749,7 @@
       <c r="R3" s="23"/>
       <c r="S3" s="23"/>
       <c r="T3" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U3" s="24"/>
     </row>
@@ -38614,7 +38758,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>242</v>
@@ -38632,7 +38776,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>28</v>
@@ -38651,7 +38795,7 @@
       <c r="R4" s="16"/>
       <c r="S4" s="16"/>
       <c r="T4" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U4" s="18"/>
     </row>
@@ -38660,7 +38804,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>242</v>
@@ -38678,7 +38822,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>28</v>
@@ -38697,7 +38841,7 @@
       <c r="R5" s="16"/>
       <c r="S5" s="16"/>
       <c r="T5" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U5" s="18"/>
     </row>
@@ -38706,7 +38850,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>242</v>
@@ -38724,7 +38868,7 @@
         <v>26</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>28</v>
@@ -38743,7 +38887,7 @@
       <c r="R6" s="16"/>
       <c r="S6" s="16"/>
       <c r="T6" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U6" s="18"/>
     </row>
@@ -38752,7 +38896,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>242</v>
@@ -38770,7 +38914,7 @@
         <v>26</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>28</v>
@@ -38789,7 +38933,7 @@
       <c r="R7" s="16"/>
       <c r="S7" s="16"/>
       <c r="T7" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U7" s="18"/>
     </row>
@@ -38798,7 +38942,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>242</v>
@@ -38816,7 +38960,7 @@
         <v>26</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>28</v>
@@ -38835,7 +38979,7 @@
       <c r="R8" s="16"/>
       <c r="S8" s="16"/>
       <c r="T8" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U8" s="18"/>
     </row>
@@ -38844,7 +38988,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>242</v>
@@ -38862,7 +39006,7 @@
         <v>26</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>28</v>
@@ -38881,7 +39025,7 @@
       <c r="R9" s="16"/>
       <c r="S9" s="16"/>
       <c r="T9" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U9" s="18"/>
     </row>
@@ -38890,7 +39034,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>242</v>
@@ -38908,7 +39052,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>28</v>
@@ -38927,7 +39071,7 @@
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
       <c r="T10" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U10" s="18"/>
     </row>
@@ -38936,7 +39080,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>242</v>
@@ -38954,7 +39098,7 @@
         <v>26</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>28</v>
@@ -38973,7 +39117,7 @@
       <c r="R11" s="16"/>
       <c r="S11" s="16"/>
       <c r="T11" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U11" s="18"/>
     </row>
@@ -38982,7 +39126,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>242</v>
@@ -39000,7 +39144,7 @@
         <v>26</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>28</v>
@@ -39019,7 +39163,7 @@
       <c r="R12" s="16"/>
       <c r="S12" s="16"/>
       <c r="T12" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U12" s="18"/>
     </row>
@@ -39028,7 +39172,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>242</v>
@@ -39046,7 +39190,7 @@
         <v>26</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>28</v>
@@ -39065,7 +39209,7 @@
       <c r="R13" s="16"/>
       <c r="S13" s="16"/>
       <c r="T13" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U13" s="18"/>
     </row>
@@ -39074,7 +39218,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>242</v>
@@ -39092,7 +39236,7 @@
         <v>26</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>28</v>
@@ -39111,7 +39255,7 @@
       <c r="R14" s="16"/>
       <c r="S14" s="16"/>
       <c r="T14" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U14" s="18"/>
     </row>
@@ -39120,7 +39264,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>242</v>
@@ -39138,7 +39282,7 @@
         <v>26</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>28</v>
@@ -39157,7 +39301,7 @@
       <c r="R15" s="16"/>
       <c r="S15" s="16"/>
       <c r="T15" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U15" s="18"/>
     </row>
@@ -39166,7 +39310,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>242</v>
@@ -39184,7 +39328,7 @@
         <v>26</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>28</v>
@@ -39203,7 +39347,7 @@
       <c r="R16" s="16"/>
       <c r="S16" s="16"/>
       <c r="T16" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U16" s="18"/>
     </row>
@@ -39212,7 +39356,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>242</v>
@@ -39230,7 +39374,7 @@
         <v>26</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>28</v>
@@ -39249,7 +39393,7 @@
       <c r="R17" s="16"/>
       <c r="S17" s="16"/>
       <c r="T17" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U17" s="18"/>
     </row>
@@ -39258,7 +39402,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>242</v>
@@ -39276,7 +39420,7 @@
         <v>26</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>28</v>
@@ -39295,7 +39439,7 @@
       <c r="R18" s="16"/>
       <c r="S18" s="16"/>
       <c r="T18" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U18" s="18"/>
     </row>
@@ -39304,7 +39448,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>242</v>
@@ -39322,7 +39466,7 @@
         <v>26</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>28</v>
@@ -39341,7 +39485,7 @@
       <c r="R19" s="16"/>
       <c r="S19" s="16"/>
       <c r="T19" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U19" s="18"/>
     </row>
@@ -39350,7 +39494,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>242</v>
@@ -39368,7 +39512,7 @@
         <v>26</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>28</v>
@@ -39387,7 +39531,7 @@
       <c r="R20" s="16"/>
       <c r="S20" s="16"/>
       <c r="T20" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U20" s="18"/>
     </row>
@@ -39396,7 +39540,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>242</v>
@@ -39414,7 +39558,7 @@
         <v>26</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>28</v>
@@ -39433,7 +39577,7 @@
       <c r="R21" s="16"/>
       <c r="S21" s="16"/>
       <c r="T21" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U21" s="18"/>
     </row>
@@ -39442,7 +39586,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>242</v>
@@ -39460,7 +39604,7 @@
         <v>26</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>28</v>
@@ -39479,7 +39623,7 @@
       <c r="R22" s="16"/>
       <c r="S22" s="16"/>
       <c r="T22" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U22" s="18"/>
     </row>
@@ -39488,7 +39632,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>242</v>
@@ -39506,7 +39650,7 @@
         <v>26</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>28</v>
@@ -39525,7 +39669,7 @@
       <c r="R23" s="16"/>
       <c r="S23" s="16"/>
       <c r="T23" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U23" s="18"/>
     </row>
@@ -39534,7 +39678,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>242</v>
@@ -39552,7 +39696,7 @@
         <v>26</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="I24" s="14" t="s">
         <v>28</v>
@@ -39571,7 +39715,7 @@
       <c r="R24" s="16"/>
       <c r="S24" s="16"/>
       <c r="T24" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U24" s="18"/>
     </row>
@@ -39580,7 +39724,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>242</v>
@@ -39598,7 +39742,7 @@
         <v>26</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="I25" s="14" t="s">
         <v>28</v>
@@ -39617,7 +39761,7 @@
       <c r="R25" s="16"/>
       <c r="S25" s="16"/>
       <c r="T25" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U25" s="18"/>
     </row>
@@ -39626,7 +39770,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>242</v>
@@ -39644,7 +39788,7 @@
         <v>26</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>28</v>
@@ -39663,7 +39807,7 @@
       <c r="R26" s="16"/>
       <c r="S26" s="16"/>
       <c r="T26" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U26" s="18"/>
     </row>
@@ -39672,7 +39816,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>242</v>
@@ -39690,7 +39834,7 @@
         <v>26</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="I27" s="14" t="s">
         <v>28</v>
@@ -39709,7 +39853,7 @@
       <c r="R27" s="16"/>
       <c r="S27" s="16"/>
       <c r="T27" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U27" s="18"/>
     </row>
@@ -39718,7 +39862,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>242</v>
@@ -39736,7 +39880,7 @@
         <v>26</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>28</v>
@@ -39755,7 +39899,7 @@
       <c r="R28" s="16"/>
       <c r="S28" s="16"/>
       <c r="T28" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U28" s="18"/>
     </row>
@@ -39764,7 +39908,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>242</v>
@@ -39782,7 +39926,7 @@
         <v>26</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="I29" s="14" t="s">
         <v>28</v>
@@ -39801,7 +39945,7 @@
       <c r="R29" s="16"/>
       <c r="S29" s="16"/>
       <c r="T29" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U29" s="18"/>
     </row>
@@ -39810,7 +39954,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>242</v>
@@ -39828,7 +39972,7 @@
         <v>26</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>28</v>
@@ -39847,7 +39991,7 @@
       <c r="R30" s="16"/>
       <c r="S30" s="16"/>
       <c r="T30" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U30" s="18"/>
     </row>
@@ -39856,7 +40000,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>242</v>
@@ -39874,7 +40018,7 @@
         <v>26</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="I31" s="14" t="s">
         <v>28</v>
@@ -39893,7 +40037,7 @@
       <c r="R31" s="16"/>
       <c r="S31" s="16"/>
       <c r="T31" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U31" s="18"/>
     </row>
@@ -39902,7 +40046,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>242</v>
@@ -39920,7 +40064,7 @@
         <v>26</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="I32" s="14" t="s">
         <v>28</v>
@@ -39939,7 +40083,7 @@
       <c r="R32" s="16"/>
       <c r="S32" s="16"/>
       <c r="T32" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U32" s="18"/>
     </row>
@@ -39948,7 +40092,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>242</v>
@@ -39966,7 +40110,7 @@
         <v>26</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="I33" s="14" t="s">
         <v>28</v>
@@ -39985,7 +40129,7 @@
       <c r="R33" s="16"/>
       <c r="S33" s="16"/>
       <c r="T33" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U33" s="18"/>
     </row>
@@ -39994,7 +40138,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>242</v>
@@ -40012,7 +40156,7 @@
         <v>26</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="I34" s="14" t="s">
         <v>28</v>
@@ -40031,7 +40175,7 @@
       <c r="R34" s="16"/>
       <c r="S34" s="16"/>
       <c r="T34" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U34" s="18"/>
     </row>
@@ -40040,7 +40184,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>242</v>
@@ -40058,7 +40202,7 @@
         <v>26</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="I35" s="14" t="s">
         <v>28</v>
@@ -40077,7 +40221,7 @@
       <c r="R35" s="16"/>
       <c r="S35" s="16"/>
       <c r="T35" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U35" s="18"/>
     </row>
@@ -40086,7 +40230,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>242</v>
@@ -40104,7 +40248,7 @@
         <v>26</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="I36" s="14" t="s">
         <v>28</v>
@@ -40123,7 +40267,7 @@
       <c r="R36" s="16"/>
       <c r="S36" s="16"/>
       <c r="T36" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U36" s="18"/>
     </row>
@@ -40132,7 +40276,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>242</v>
@@ -40150,7 +40294,7 @@
         <v>26</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="I37" s="14" t="s">
         <v>28</v>
@@ -40169,7 +40313,7 @@
       <c r="R37" s="16"/>
       <c r="S37" s="16"/>
       <c r="T37" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U37" s="18"/>
     </row>
@@ -40178,7 +40322,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>242</v>
@@ -40196,7 +40340,7 @@
         <v>26</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="I38" s="14" t="s">
         <v>28</v>
@@ -40215,7 +40359,7 @@
       <c r="R38" s="16"/>
       <c r="S38" s="16"/>
       <c r="T38" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U38" s="18"/>
     </row>
@@ -40224,7 +40368,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>242</v>
@@ -40242,7 +40386,7 @@
         <v>26</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="I39" s="21" t="s">
         <v>28</v>
@@ -40261,7 +40405,7 @@
       <c r="R39" s="23"/>
       <c r="S39" s="23"/>
       <c r="T39" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U39" s="24"/>
     </row>
@@ -40270,7 +40414,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>242</v>
@@ -40288,7 +40432,7 @@
         <v>26</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="I40" s="14" t="s">
         <v>28</v>
@@ -40307,7 +40451,7 @@
       <c r="R40" s="16"/>
       <c r="S40" s="16"/>
       <c r="T40" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U40" s="18"/>
     </row>
@@ -40316,7 +40460,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>242</v>
@@ -40334,7 +40478,7 @@
         <v>26</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="I41" s="14" t="s">
         <v>28</v>
@@ -40353,7 +40497,7 @@
       <c r="R41" s="16"/>
       <c r="S41" s="16"/>
       <c r="T41" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U41" s="18"/>
     </row>
@@ -40362,7 +40506,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>242</v>
@@ -40380,7 +40524,7 @@
         <v>26</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="I42" s="14" t="s">
         <v>28</v>
@@ -40399,7 +40543,7 @@
       <c r="R42" s="16"/>
       <c r="S42" s="16"/>
       <c r="T42" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U42" s="18"/>
     </row>
@@ -40408,7 +40552,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>242</v>
@@ -40426,7 +40570,7 @@
         <v>26</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="I43" s="14" t="s">
         <v>28</v>
@@ -40445,7 +40589,7 @@
       <c r="R43" s="16"/>
       <c r="S43" s="16"/>
       <c r="T43" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U43" s="18"/>
     </row>
@@ -40454,7 +40598,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>242</v>
@@ -40472,7 +40616,7 @@
         <v>26</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="I44" s="14" t="s">
         <v>28</v>
@@ -40491,7 +40635,7 @@
       <c r="R44" s="16"/>
       <c r="S44" s="16"/>
       <c r="T44" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U44" s="18"/>
     </row>
@@ -40500,7 +40644,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>242</v>
@@ -40518,7 +40662,7 @@
         <v>26</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="I45" s="14" t="s">
         <v>28</v>
@@ -40537,7 +40681,7 @@
       <c r="R45" s="16"/>
       <c r="S45" s="16"/>
       <c r="T45" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U45" s="18"/>
     </row>
@@ -40546,7 +40690,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>242</v>
@@ -40564,7 +40708,7 @@
         <v>26</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="I46" s="14" t="s">
         <v>28</v>
@@ -40583,7 +40727,7 @@
       <c r="R46" s="16"/>
       <c r="S46" s="16"/>
       <c r="T46" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U46" s="18"/>
     </row>
@@ -40592,7 +40736,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>242</v>
@@ -40610,7 +40754,7 @@
         <v>26</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="I47" s="14" t="s">
         <v>28</v>
@@ -40629,7 +40773,7 @@
       <c r="R47" s="16"/>
       <c r="S47" s="16"/>
       <c r="T47" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U47" s="18"/>
     </row>
@@ -40638,7 +40782,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>242</v>
@@ -40656,7 +40800,7 @@
         <v>26</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="I48" s="14" t="s">
         <v>28</v>
@@ -40675,7 +40819,7 @@
       <c r="R48" s="16"/>
       <c r="S48" s="16"/>
       <c r="T48" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U48" s="18"/>
     </row>
@@ -40684,7 +40828,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="C49" s="14" t="s">
         <v>242</v>
@@ -40702,7 +40846,7 @@
         <v>26</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="I49" s="14" t="s">
         <v>28</v>
@@ -40721,7 +40865,7 @@
       <c r="R49" s="16"/>
       <c r="S49" s="16"/>
       <c r="T49" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U49" s="18"/>
     </row>
@@ -40730,7 +40874,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>242</v>
@@ -40748,7 +40892,7 @@
         <v>26</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="I50" s="14" t="s">
         <v>28</v>
@@ -40767,7 +40911,7 @@
       <c r="R50" s="16"/>
       <c r="S50" s="16"/>
       <c r="T50" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U50" s="18"/>
     </row>
@@ -40776,7 +40920,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>242</v>
@@ -40794,7 +40938,7 @@
         <v>26</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="I51" s="14" t="s">
         <v>28</v>
@@ -40813,7 +40957,7 @@
       <c r="R51" s="16"/>
       <c r="S51" s="16"/>
       <c r="T51" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U51" s="18"/>
     </row>
@@ -40822,7 +40966,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>242</v>
@@ -40840,7 +40984,7 @@
         <v>26</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="I52" s="14" t="s">
         <v>28</v>
@@ -40859,7 +41003,7 @@
       <c r="R52" s="16"/>
       <c r="S52" s="16"/>
       <c r="T52" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U52" s="18"/>
     </row>
@@ -40868,7 +41012,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>242</v>
@@ -40886,7 +41030,7 @@
         <v>26</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="I53" s="14" t="s">
         <v>28</v>
@@ -40905,7 +41049,7 @@
       <c r="R53" s="16"/>
       <c r="S53" s="16"/>
       <c r="T53" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U53" s="18"/>
     </row>
@@ -40914,7 +41058,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>242</v>
@@ -40932,7 +41076,7 @@
         <v>26</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="I54" s="14" t="s">
         <v>28</v>
@@ -40951,7 +41095,7 @@
       <c r="R54" s="16"/>
       <c r="S54" s="16"/>
       <c r="T54" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U54" s="18"/>
     </row>
@@ -40960,7 +41104,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>242</v>
@@ -40978,7 +41122,7 @@
         <v>26</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="I55" s="14" t="s">
         <v>28</v>
@@ -40997,7 +41141,7 @@
       <c r="R55" s="16"/>
       <c r="S55" s="16"/>
       <c r="T55" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U55" s="18"/>
     </row>
@@ -41006,7 +41150,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>242</v>
@@ -41024,7 +41168,7 @@
         <v>26</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="I56" s="14" t="s">
         <v>28</v>
@@ -41043,7 +41187,7 @@
       <c r="R56" s="16"/>
       <c r="S56" s="16"/>
       <c r="T56" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U56" s="18"/>
     </row>
@@ -41052,7 +41196,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>242</v>
@@ -41070,7 +41214,7 @@
         <v>26</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="I57" s="14" t="s">
         <v>28</v>
@@ -41089,7 +41233,7 @@
       <c r="R57" s="16"/>
       <c r="S57" s="16"/>
       <c r="T57" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U57" s="18"/>
     </row>
@@ -41098,7 +41242,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>242</v>
@@ -41116,7 +41260,7 @@
         <v>26</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="I58" s="14" t="s">
         <v>28</v>
@@ -41135,7 +41279,7 @@
       <c r="R58" s="16"/>
       <c r="S58" s="16"/>
       <c r="T58" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U58" s="18"/>
     </row>
@@ -41144,7 +41288,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>242</v>
@@ -41162,7 +41306,7 @@
         <v>26</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="I59" s="14" t="s">
         <v>28</v>
@@ -41181,7 +41325,7 @@
       <c r="R59" s="16"/>
       <c r="S59" s="16"/>
       <c r="T59" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U59" s="18"/>
     </row>
@@ -41190,7 +41334,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>242</v>
@@ -41208,7 +41352,7 @@
         <v>26</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="I60" s="14" t="s">
         <v>28</v>
@@ -41227,7 +41371,7 @@
       <c r="R60" s="16"/>
       <c r="S60" s="16"/>
       <c r="T60" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U60" s="18"/>
     </row>
@@ -41236,7 +41380,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>242</v>
@@ -41254,7 +41398,7 @@
         <v>26</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="I61" s="14" t="s">
         <v>28</v>
@@ -41273,7 +41417,7 @@
       <c r="R61" s="16"/>
       <c r="S61" s="16"/>
       <c r="T61" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U61" s="18"/>
     </row>
@@ -41282,7 +41426,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>242</v>
@@ -41300,7 +41444,7 @@
         <v>26</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="I62" s="14" t="s">
         <v>28</v>
@@ -41319,7 +41463,7 @@
       <c r="R62" s="16"/>
       <c r="S62" s="16"/>
       <c r="T62" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U62" s="18"/>
     </row>
@@ -41328,7 +41472,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>242</v>
@@ -41346,7 +41490,7 @@
         <v>26</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="I63" s="14" t="s">
         <v>28</v>
@@ -41365,7 +41509,7 @@
       <c r="R63" s="16"/>
       <c r="S63" s="16"/>
       <c r="T63" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U63" s="18"/>
     </row>
@@ -41374,7 +41518,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>242</v>
@@ -41392,7 +41536,7 @@
         <v>26</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="I64" s="14" t="s">
         <v>28</v>
@@ -41411,7 +41555,7 @@
       <c r="R64" s="16"/>
       <c r="S64" s="16"/>
       <c r="T64" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U64" s="18"/>
     </row>
@@ -41420,7 +41564,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>242</v>
@@ -41438,7 +41582,7 @@
         <v>26</v>
       </c>
       <c r="H65" s="14" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="I65" s="14" t="s">
         <v>28</v>
@@ -41457,7 +41601,7 @@
       <c r="R65" s="16"/>
       <c r="S65" s="16"/>
       <c r="T65" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U65" s="18"/>
     </row>
@@ -41466,7 +41610,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>242</v>
@@ -41484,7 +41628,7 @@
         <v>26</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="I66" s="14" t="s">
         <v>28</v>
@@ -41503,7 +41647,7 @@
       <c r="R66" s="16"/>
       <c r="S66" s="16"/>
       <c r="T66" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U66" s="18"/>
     </row>
@@ -41512,7 +41656,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>242</v>
@@ -41530,7 +41674,7 @@
         <v>26</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="I67" s="14" t="s">
         <v>28</v>
@@ -41549,7 +41693,7 @@
       <c r="R67" s="16"/>
       <c r="S67" s="16"/>
       <c r="T67" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U67" s="18"/>
     </row>
@@ -41558,7 +41702,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>242</v>
@@ -41576,7 +41720,7 @@
         <v>26</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="I68" s="14" t="s">
         <v>28</v>
@@ -41595,7 +41739,7 @@
       <c r="R68" s="16"/>
       <c r="S68" s="16"/>
       <c r="T68" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U68" s="18"/>
     </row>
@@ -41604,7 +41748,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>242</v>
@@ -41622,7 +41766,7 @@
         <v>26</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="I69" s="14" t="s">
         <v>28</v>
@@ -41641,7 +41785,7 @@
       <c r="R69" s="16"/>
       <c r="S69" s="16"/>
       <c r="T69" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U69" s="18"/>
     </row>
@@ -41650,7 +41794,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>242</v>
@@ -41668,7 +41812,7 @@
         <v>26</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="I70" s="14" t="s">
         <v>28</v>
@@ -41687,7 +41831,7 @@
       <c r="R70" s="16"/>
       <c r="S70" s="16"/>
       <c r="T70" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U70" s="18"/>
     </row>
@@ -41696,7 +41840,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>242</v>
@@ -41714,7 +41858,7 @@
         <v>26</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="I71" s="14" t="s">
         <v>28</v>
@@ -41733,7 +41877,7 @@
       <c r="R71" s="16"/>
       <c r="S71" s="16"/>
       <c r="T71" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U71" s="18"/>
     </row>
@@ -41742,7 +41886,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>242</v>
@@ -41760,7 +41904,7 @@
         <v>26</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="I72" s="14" t="s">
         <v>28</v>
@@ -41779,7 +41923,7 @@
       <c r="R72" s="16"/>
       <c r="S72" s="16"/>
       <c r="T72" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U72" s="18"/>
     </row>
@@ -41788,7 +41932,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>242</v>
@@ -41806,7 +41950,7 @@
         <v>26</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="I73" s="14" t="s">
         <v>28</v>
@@ -41825,7 +41969,7 @@
       <c r="R73" s="16"/>
       <c r="S73" s="16"/>
       <c r="T73" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U73" s="18"/>
     </row>
@@ -41834,7 +41978,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>242</v>
@@ -41852,7 +41996,7 @@
         <v>26</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="I74" s="14" t="s">
         <v>28</v>
@@ -41871,7 +42015,7 @@
       <c r="R74" s="16"/>
       <c r="S74" s="16"/>
       <c r="T74" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U74" s="18"/>
     </row>
@@ -41880,7 +42024,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>242</v>
@@ -41898,7 +42042,7 @@
         <v>26</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="I75" s="14" t="s">
         <v>28</v>
@@ -41917,7 +42061,7 @@
       <c r="R75" s="16"/>
       <c r="S75" s="16"/>
       <c r="T75" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U75" s="18"/>
     </row>
@@ -41926,7 +42070,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>242</v>
@@ -41944,7 +42088,7 @@
         <v>26</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="I76" s="14" t="s">
         <v>28</v>
@@ -41963,7 +42107,7 @@
       <c r="R76" s="16"/>
       <c r="S76" s="16"/>
       <c r="T76" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U76" s="18"/>
     </row>
@@ -41972,7 +42116,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>242</v>
@@ -41990,7 +42134,7 @@
         <v>26</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="I77" s="14" t="s">
         <v>28</v>
@@ -42009,7 +42153,7 @@
       <c r="R77" s="16"/>
       <c r="S77" s="16"/>
       <c r="T77" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U77" s="18"/>
     </row>
@@ -42018,7 +42162,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>242</v>
@@ -42036,7 +42180,7 @@
         <v>26</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="I78" s="14" t="s">
         <v>28</v>
@@ -42055,7 +42199,7 @@
       <c r="R78" s="16"/>
       <c r="S78" s="16"/>
       <c r="T78" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U78" s="18"/>
     </row>
@@ -42064,7 +42208,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="C79" s="14" t="s">
         <v>242</v>
@@ -42082,7 +42226,7 @@
         <v>26</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="I79" s="14" t="s">
         <v>28</v>
@@ -42101,7 +42245,7 @@
       <c r="R79" s="16"/>
       <c r="S79" s="16"/>
       <c r="T79" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U79" s="18"/>
     </row>
@@ -42110,7 +42254,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>242</v>
@@ -42128,7 +42272,7 @@
         <v>26</v>
       </c>
       <c r="H80" s="14" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="I80" s="14" t="s">
         <v>28</v>
@@ -42147,7 +42291,7 @@
       <c r="R80" s="16"/>
       <c r="S80" s="16"/>
       <c r="T80" s="16" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U80" s="18"/>
     </row>
@@ -42156,7 +42300,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="C81" s="21" t="s">
         <v>242</v>
@@ -42174,7 +42318,7 @@
         <v>26</v>
       </c>
       <c r="H81" s="21" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="I81" s="21" t="s">
         <v>28</v>
@@ -42193,7 +42337,7 @@
       <c r="R81" s="23"/>
       <c r="S81" s="23"/>
       <c r="T81" s="23" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="U81" s="24"/>
     </row>
@@ -42301,7 +42445,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>22</v>
@@ -42313,13 +42457,13 @@
         <v>24</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>28</v>
@@ -42357,7 +42501,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>22</v>
@@ -42369,13 +42513,13 @@
         <v>24</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="I3" s="35" t="s">
         <v>28</v>
@@ -42413,7 +42557,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>22</v>
@@ -42425,13 +42569,13 @@
         <v>24</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="I4" s="29" t="s">
         <v>28</v>
@@ -42469,7 +42613,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>22</v>
@@ -42490,7 +42634,7 @@
         <v>334</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="J5" s="36" t="str">
         <f t="shared" si="0"/>
@@ -42525,7 +42669,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>242</v>
@@ -42543,7 +42687,7 @@
         <v>26</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="I6" s="35" t="s">
         <v>28</v>
@@ -42581,25 +42725,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="I7" s="29" t="s">
         <v>34</v>
@@ -42637,25 +42781,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="68" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="C8" s="69" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E8" s="69" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="69" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="I8" s="69" t="s">
         <v>40</v>
@@ -42793,19 +42937,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
+        <v>624</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>620</v>
       </c>
-      <c r="C2" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>616</v>
-      </c>
       <c r="E2" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>26</v>
@@ -42855,25 +42999,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G3" s="29">
         <v>1</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>28</v>
@@ -42901,7 +43045,7 @@
         <v>30</v>
       </c>
       <c r="P3" s="31" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="Q3" s="31" t="s">
         <v>345</v>
@@ -42925,25 +43069,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G4" s="29">
         <v>1</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="I4" s="29" t="s">
         <v>28</v>
@@ -42971,7 +43115,7 @@
         <v>30</v>
       </c>
       <c r="P4" s="31" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="Q4" s="31" t="s">
         <v>345</v>
@@ -42995,25 +43139,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G5" s="29">
         <v>1</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="I5" s="29" t="s">
         <v>28</v>
@@ -43057,25 +43201,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G6" s="29">
         <v>1</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="I6" s="29" t="s">
         <v>28</v>
@@ -43119,28 +43263,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G7" s="35">
         <v>1</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="J7" s="36" t="str">
         <f t="shared" si="0"/>
@@ -43181,28 +43325,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G8" s="35">
         <v>1</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="J8" s="36" t="str">
         <f t="shared" si="0"/>
@@ -43243,28 +43387,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E9" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G9" s="35">
         <v>1</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
       <c r="I9" s="35" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="J9" s="36" t="str">
         <f t="shared" si="0"/>
@@ -43305,28 +43449,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="C10" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G10" s="35">
         <v>1</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="J10" s="36" t="str">
         <f t="shared" si="0"/>
@@ -43367,25 +43511,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G11" s="29">
         <v>1</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="I11" s="29" t="s">
         <v>28</v>
@@ -43429,25 +43573,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G12" s="29">
         <v>1</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="I12" s="29" t="s">
         <v>28</v>
@@ -43491,13 +43635,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>24</v>
@@ -43509,7 +43653,7 @@
         <v>26</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="I13" s="29" t="s">
         <v>28</v>
@@ -43553,25 +43697,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G14" s="35">
         <v>2</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="I14" s="35" t="s">
         <v>28</v>
@@ -43609,25 +43753,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G15" s="35">
         <v>2</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="I15" s="35" t="s">
         <v>28</v>
@@ -43665,25 +43809,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G16" s="35">
         <v>2</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="I16" s="35" t="s">
         <v>28</v>
@@ -43721,25 +43865,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="C17" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G17" s="35">
         <v>2</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="I17" s="35" t="s">
         <v>28</v>
@@ -43777,19 +43921,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="C18" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E18" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G18" s="35">
         <v>2</v>
@@ -43829,19 +43973,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="C19" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G19" s="35">
         <v>2</v>
@@ -43881,19 +44025,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="C20" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E20" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G20" s="35">
         <v>2</v>
@@ -43933,19 +44077,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="C21" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E21" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G21" s="35">
         <v>2</v>
@@ -43985,19 +44129,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
       <c r="C22" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G22" s="35">
         <v>2</v>
@@ -44037,19 +44181,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="C23" s="41" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G23" s="41">
         <v>2</v>

</xml_diff>

<commit_message>
Fix interlock hardware failure scan field
</commit_message>
<xml_diff>
--- a/etc/Storage Ring A Interlock EPICS.xlsx
+++ b/etc/Storage Ring A Interlock EPICS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25506"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AD58B01-8D61-4BA9-A5C5-6CF8D4725EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB09735E-1252-416B-A5D1-B79C10169BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="90" yWindow="1560" windowWidth="20400" windowHeight="9480" tabRatio="719" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44870,8 +44870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC2DBB1-5D49-469C-81C7-E7BFC2EB4E9C}">
   <dimension ref="A1:U229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -45408,7 +45408,7 @@
         <v>636</v>
       </c>
       <c r="T9" s="87" t="s">
-        <v>635</v>
+        <v>31</v>
       </c>
       <c r="U9" s="88" t="s">
         <v>635</v>

</xml_diff>